<commit_message>
update output genomics computation
</commit_message>
<xml_diff>
--- a/templates/dataplant/4COM04_GenomeAssembly.xlsx
+++ b/templates/dataplant/4COM04_GenomeAssembly.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin\source\repos\SWATE_templates\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martin\Documents\GitHub\Swate-templates_FORK\templates\dataplant\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9F624C4-0DBE-486C-AFE8-CE8906DEED6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C90DBDBB-A74E-4C93-AE15-D889F4375824}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="19110" windowHeight="12450" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6165" yWindow="2340" windowWidth="22785" windowHeight="14535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="4COM04_GenomeAssembly" sheetId="1" r:id="rId1"/>
@@ -241,9 +241,6 @@
     <t>Term Accession Number (NFDI4PSO:0000027)</t>
   </si>
   <si>
-    <t>Data File Name</t>
-  </si>
-  <si>
     <t>Id</t>
   </si>
   <si>
@@ -575,13 +572,16 @@
   </si>
   <si>
     <t>Authors Role Term Source REF</t>
+  </si>
+  <si>
+    <t>Derived Data File</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -596,12 +596,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="6">
@@ -733,7 +727,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -771,11 +765,16 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -836,7 +835,7 @@
     <tableColumn id="36" xr3:uid="{BABEB0E1-C070-4A62-BA72-FDA195146EFD}" name="Parameter [Processed data file format]"/>
     <tableColumn id="37" xr3:uid="{8611E0EA-5557-4A72-9D69-AAF4C5BBCA3F}" name="Term Source REF (NFDI4PSO:0000027)"/>
     <tableColumn id="38" xr3:uid="{77A26896-8666-47F3-8757-1DBF8D855FA0}" name="Term Accession Number (NFDI4PSO:0000027)"/>
-    <tableColumn id="39" xr3:uid="{711C7885-CD0B-42CC-9663-F97199B54258}" name="Data File Name"/>
+    <tableColumn id="2" xr3:uid="{37AAA820-E44D-492C-A2D8-56248E8B1009}" name="Derived Data File" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1140,7 +1139,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="659" row="2">
+  <wetp:taskpane dockstate="right" visibility="0" width="350" row="3">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
   <wetp:taskpane dockstate="right" visibility="0" width="656" row="2">
@@ -1173,48 +1172,50 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AL2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
+      <selection activeCell="AI2" sqref="AI2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="36.7109375" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="34.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="36.7109375" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="42" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="42.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="36.7109375" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="45.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="46.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="36.7109375" hidden="1" customWidth="1"/>
     <col min="13" max="13" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="57" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="57.42578125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="36.7109375" hidden="1" customWidth="1"/>
     <col min="16" max="16" width="46.5703125" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="41.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="41.7109375" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="30.85546875" hidden="1" customWidth="1"/>
     <col min="19" max="19" width="37.85546875" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="48.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="49.140625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="36.7109375" hidden="1" customWidth="1"/>
     <col min="22" max="22" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="23" max="23" width="37.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="38" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="30.85546875" hidden="1" customWidth="1"/>
     <col min="25" max="25" width="37.85546875" hidden="1" customWidth="1"/>
-    <col min="26" max="26" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="30.7109375" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="30.85546875" hidden="1" customWidth="1"/>
     <col min="28" max="28" width="37.85546875" hidden="1" customWidth="1"/>
-    <col min="29" max="29" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="28.42578125" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="36.7109375" hidden="1" customWidth="1"/>
     <col min="31" max="31" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="32" max="32" width="41" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="41.28515625" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="36.7109375" hidden="1" customWidth="1"/>
     <col min="34" max="34" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="35" max="35" width="38.140625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="38.42578125" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="36.7109375" hidden="1" customWidth="1"/>
     <col min="37" max="37" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="38" max="38" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="18.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:38" x14ac:dyDescent="0.25">
@@ -1330,19 +1331,20 @@
         <v>36</v>
       </c>
       <c r="AL1" t="s">
-        <v>37</v>
+        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.25">
       <c r="N2" t="s">
+        <v>139</v>
+      </c>
+      <c r="O2" t="s">
+        <v>89</v>
+      </c>
+      <c r="P2" t="s">
         <v>140</v>
       </c>
-      <c r="O2" t="s">
-        <v>90</v>
-      </c>
-      <c r="P2" t="s">
-        <v>141</v>
-      </c>
+      <c r="AL2" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1356,7 +1358,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2198836-D18B-4D0A-A514-00A7EC4AFC3D}">
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
@@ -1368,55 +1370,55 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -1424,19 +1426,19 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B8" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>65</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>66</v>
       </c>
       <c r="D8" s="8"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -1444,7 +1446,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
@@ -1452,7 +1454,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
@@ -1460,21 +1462,21 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B12" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C12" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="D12" s="8" t="s">
         <v>68</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -1482,7 +1484,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
@@ -1490,7 +1492,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
@@ -1498,35 +1500,35 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B16" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C16" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="D16" s="8" t="s">
         <v>71</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B17" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C17" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="D17" s="6" t="s">
         <v>74</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
@@ -1534,7 +1536,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
@@ -1542,7 +1544,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
@@ -1550,7 +1552,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
@@ -1558,7 +1560,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
@@ -1566,7 +1568,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
@@ -1574,7 +1576,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
@@ -1582,7 +1584,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
@@ -1590,7 +1592,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
@@ -1598,7 +1600,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B27" s="9"/>
       <c r="C27" s="9"/>
@@ -1634,40 +1636,40 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="C1" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="D1" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="E1" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="F1" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="G1" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="H1" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="I1" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="J1" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="K1" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="L1" s="11" t="s">
         <v>86</v>
-      </c>
-      <c r="L1" s="11" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -1675,19 +1677,19 @@
         <v>0</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
@@ -1698,31 +1700,31 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G3" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="H3" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="I3" s="12" t="s">
         <v>119</v>
-      </c>
-      <c r="I3" s="12" t="s">
-        <v>120</v>
       </c>
       <c r="J3" s="12"/>
       <c r="K3" s="12"/>
@@ -1733,28 +1735,28 @@
         <v>1</v>
       </c>
       <c r="B4" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="C4" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="D4" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="D4" s="12" t="s">
-        <v>91</v>
-      </c>
       <c r="E4" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G4" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="H4" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="H4" s="12" t="s">
-        <v>122</v>
-      </c>
       <c r="I4" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J4" s="12"/>
       <c r="K4" s="12"/>
@@ -1765,24 +1767,24 @@
         <v>4</v>
       </c>
       <c r="B5" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="D5" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="C5" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>93</v>
-      </c>
       <c r="E5" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
       <c r="I5" s="12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J5" s="12"/>
       <c r="K5" s="12"/>
@@ -1793,24 +1795,24 @@
         <v>7</v>
       </c>
       <c r="B6" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="D6" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="C6" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>95</v>
-      </c>
       <c r="E6" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G6" s="12"/>
       <c r="H6" s="12"/>
       <c r="I6" s="12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J6" s="12"/>
       <c r="K6" s="12"/>
@@ -1821,24 +1823,24 @@
         <v>10</v>
       </c>
       <c r="B7" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="D7" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="C7" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>97</v>
-      </c>
       <c r="E7" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G7" s="12"/>
       <c r="H7" s="12"/>
       <c r="I7" s="12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J7" s="12"/>
       <c r="K7" s="12"/>
@@ -1849,28 +1851,28 @@
         <v>13</v>
       </c>
       <c r="B8" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="D8" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="C8" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>99</v>
-      </c>
       <c r="E8" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G8" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="H8" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="H8" s="12" t="s">
+      <c r="I8" s="12" t="s">
         <v>125</v>
-      </c>
-      <c r="I8" s="12" t="s">
-        <v>126</v>
       </c>
       <c r="J8" s="12"/>
       <c r="K8" s="12"/>
@@ -1881,28 +1883,28 @@
         <v>16</v>
       </c>
       <c r="B9" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="C9" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="D9" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="D9" s="12" t="s">
-        <v>102</v>
-      </c>
       <c r="E9" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G9" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="H9" s="12" t="s">
         <v>127</v>
       </c>
-      <c r="H9" s="12" t="s">
-        <v>128</v>
-      </c>
       <c r="I9" s="12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J9" s="12"/>
       <c r="K9" s="12"/>
@@ -1913,28 +1915,28 @@
         <v>19</v>
       </c>
       <c r="B10" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="D10" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="C10" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>104</v>
-      </c>
       <c r="E10" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G10" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="H10" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="H10" s="12" t="s">
-        <v>130</v>
-      </c>
       <c r="I10" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J10" s="12"/>
       <c r="K10" s="12"/>
@@ -1945,28 +1947,28 @@
         <v>22</v>
       </c>
       <c r="B11" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="D11" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="C11" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>106</v>
-      </c>
       <c r="E11" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G11" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="H11" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="H11" s="12" t="s">
+      <c r="I11" s="12" t="s">
         <v>132</v>
-      </c>
-      <c r="I11" s="12" t="s">
-        <v>133</v>
       </c>
       <c r="J11" s="12"/>
       <c r="K11" s="12"/>
@@ -1977,28 +1979,28 @@
         <v>25</v>
       </c>
       <c r="B12" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="D12" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="C12" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="D12" s="12" t="s">
-        <v>108</v>
-      </c>
       <c r="E12" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G12" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="H12" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="H12" s="12" t="s">
-        <v>135</v>
-      </c>
       <c r="I12" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J12" s="12"/>
       <c r="K12" s="12"/>
@@ -2009,19 +2011,19 @@
         <v>28</v>
       </c>
       <c r="B13" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="D13" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="C13" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="D13" s="12" t="s">
-        <v>110</v>
-      </c>
       <c r="E13" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G13" s="12"/>
       <c r="H13" s="12"/>
@@ -2035,28 +2037,28 @@
         <v>31</v>
       </c>
       <c r="B14" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="D14" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="C14" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="D14" s="12" t="s">
-        <v>112</v>
-      </c>
       <c r="E14" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G14" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="H14" s="12" t="s">
         <v>136</v>
       </c>
-      <c r="H14" s="12" t="s">
-        <v>137</v>
-      </c>
       <c r="I14" s="12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J14" s="12"/>
       <c r="K14" s="12"/>
@@ -2064,31 +2066,31 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="B15" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="C15" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="D15" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="C15" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="D15" s="12" t="s">
-        <v>115</v>
-      </c>
       <c r="E15" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G15" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="H15" s="12" t="s">
         <v>138</v>
       </c>
-      <c r="H15" s="12" t="s">
-        <v>139</v>
-      </c>
       <c r="I15" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J15" s="12"/>
       <c r="K15" s="12"/>
@@ -2099,24 +2101,24 @@
         <v>34</v>
       </c>
       <c r="B16" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="D16" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="C16" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="D16" s="12" t="s">
-        <v>117</v>
-      </c>
       <c r="E16" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G16" s="12"/>
       <c r="H16" s="12"/>
       <c r="I16" s="12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J16" s="12"/>
       <c r="K16" s="12"/>

</xml_diff>

<commit_message>
replace nfdi4pso terms in genome assembly template
</commit_message>
<xml_diff>
--- a/templates/dataplant/4COM04_GenomeAssembly.xlsx
+++ b/templates/dataplant/4COM04_GenomeAssembly.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martin\Documents\GitHub\Swate-templates_FORK\templates\dataplant\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stella Eggels\sciebo - Eggels, Stella (s.eggels@fz-juelich.de)@fz-juelich.sciebo.de\SE\DataPLANT\ARCs und SWATE\ersatz von nfdi4pso\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C90DBDBB-A74E-4C93-AE15-D889F4375824}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{828227F5-40BA-4FC4-9040-C62E6D82AD2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6165" yWindow="2340" windowWidth="22785" windowHeight="14535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="4COM04_GenomeAssembly" sheetId="1" r:id="rId1"/>
@@ -51,75 +51,75 @@
   <commentList>
     <comment ref="A1" authorId="0" shapeId="0" xr:uid="{1B82A122-B7DC-4A5B-92B7-EFF54693A4C6}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
     The unique identifier of this template. It will be auto generated.
-Reply:
+Antwort:
     id=11b23480-80a8-4d95-a2bb-b3e9c7d53a23</t>
       </text>
     </comment>
     <comment ref="A2" authorId="1" shapeId="0" xr:uid="{7F2B0E6D-7667-4BBE-84EF-E94F714AF9D5}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
     The name of the Swate template.</t>
       </text>
     </comment>
     <comment ref="A3" authorId="2" shapeId="0" xr:uid="{55280B2E-9540-497C-8359-55487A5C5B18}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
     The current version of this template in SemVer notation.</t>
       </text>
     </comment>
     <comment ref="A4" authorId="3" shapeId="0" xr:uid="{F0D435E2-551F-45A7-BCE6-994AC7ADA3CA}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
     The description of this template. Use few sentences for succinctness.</t>
       </text>
     </comment>
     <comment ref="A5" authorId="4" shapeId="0" xr:uid="{E6BCAC0A-6199-4E14-8166-0207D5BB43BA}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
     The name of the template associated organisation. "DataPLANT" will trigger the "DataPLANT" batch of honor for the template.</t>
       </text>
     </comment>
     <comment ref="A6" authorId="5" shapeId="0" xr:uid="{60BEB3E6-604B-45C4-BB34-C8023C7A5426}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
     The name of the Swate annotation table in the workbook of the template's excel file.</t>
       </text>
     </comment>
     <comment ref="A7" authorId="6" shapeId="0" xr:uid="{3F4F0D99-C656-496E-AC9C-D9F60E63A964}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
     A list of all ERs (endpoint repositories) targeted with this template. ERs are realized as Terms: &lt;term ref here&gt;</t>
       </text>
     </comment>
     <comment ref="A11" authorId="7" shapeId="0" xr:uid="{9FE4B02B-3403-489E-8E1F-763CB8E6BEEA}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
     A list of all tags associated with this template. Tags are realized as Terms: &lt;term ref here&gt;</t>
       </text>
     </comment>
     <comment ref="A15" authorId="8" shapeId="0" xr:uid="{CDC4E02C-8CF8-4363-A689-0DE050A2C5DC}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
     The author(s) of this template.</t>
       </text>
     </comment>
@@ -128,7 +128,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="150">
   <si>
     <t>Source Name</t>
   </si>
@@ -136,48 +136,6 @@
     <t>Parameter [BioSample Accession Number]</t>
   </si>
   <si>
-    <t>Term Source REF (NFDI4PSO:0000078)</t>
-  </si>
-  <si>
-    <t>Term Accession Number (NFDI4PSO:0000078)</t>
-  </si>
-  <si>
-    <t>Parameter [Data filtering software]</t>
-  </si>
-  <si>
-    <t>Term Source REF (NFDI4PSO:0000023)</t>
-  </si>
-  <si>
-    <t>Term Accession Number (NFDI4PSO:0000023)</t>
-  </si>
-  <si>
-    <t>Parameter [Data filtering software version]</t>
-  </si>
-  <si>
-    <t>Term Source REF (NFDI4PSO:0000024)</t>
-  </si>
-  <si>
-    <t>Term Accession Number (NFDI4PSO:0000024)</t>
-  </si>
-  <si>
-    <t>Parameter [Data filtering Software Parameters]</t>
-  </si>
-  <si>
-    <t>Term Source REF (NFDI4PSO:0000025)</t>
-  </si>
-  <si>
-    <t>Term Accession Number (NFDI4PSO:0000025)</t>
-  </si>
-  <si>
-    <t>Parameter [Next generation sequencing instrument model]</t>
-  </si>
-  <si>
-    <t>Term Source REF (NFDI4PSO:0000040)</t>
-  </si>
-  <si>
-    <t>Term Accession Number (NFDI4PSO:0000040)</t>
-  </si>
-  <si>
     <t>Parameter [sequence assembly algorithm]</t>
   </si>
   <si>
@@ -187,15 +145,6 @@
     <t>Term Accession Number (OBI:0001522)</t>
   </si>
   <si>
-    <t>Parameter [Sequence assembly algorithm version]</t>
-  </si>
-  <si>
-    <t>Term Source REF (NFDI4PSO:0000060)</t>
-  </si>
-  <si>
-    <t>Term Accession Number (NFDI4PSO:0000060)</t>
-  </si>
-  <si>
     <t>Parameter [sequence assembly name]</t>
   </si>
   <si>
@@ -214,33 +163,9 @@
     <t>Term Accession Number (OBI:0001939)</t>
   </si>
   <si>
-    <t>Parameter [Genome status]</t>
-  </si>
-  <si>
-    <t>Term Source REF (NFDI4PSO:0000061)</t>
-  </si>
-  <si>
-    <t>Term Accession Number (NFDI4PSO:0000061)</t>
-  </si>
-  <si>
-    <t>Parameter [Genome reference sequence]</t>
-  </si>
-  <si>
-    <t>Term Source REF (NFDI4PSO:0000026)</t>
-  </si>
-  <si>
-    <t>Term Accession Number (NFDI4PSO:0000026)</t>
-  </si>
-  <si>
     <t>Parameter [Processed data file format]</t>
   </si>
   <si>
-    <t>Term Source REF (NFDI4PSO:0000027)</t>
-  </si>
-  <si>
-    <t>Term Accession Number (NFDI4PSO:0000027)</t>
-  </si>
-  <si>
     <t>Id</t>
   </si>
   <si>
@@ -394,39 +319,9 @@
     <t>Sample Name</t>
   </si>
   <si>
-    <t>NFDI4PSO:0000078</t>
-  </si>
-  <si>
     <t>NFDI4PSO</t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/NFDI4PSO_0000078</t>
-  </si>
-  <si>
-    <t>NFDI4PSO:0000023</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NFDI4PSO_0000023</t>
-  </si>
-  <si>
-    <t>NFDI4PSO:0000024</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NFDI4PSO_0000024</t>
-  </si>
-  <si>
-    <t>NFDI4PSO:0000025</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NFDI4PSO_0000025</t>
-  </si>
-  <si>
-    <t>NFDI4PSO:0000040</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NFDI4PSO_0000040</t>
-  </si>
-  <si>
     <t>OBI:0001522</t>
   </si>
   <si>
@@ -436,12 +331,6 @@
     <t>http://purl.obolibrary.org/obo/OBI_0001522</t>
   </si>
   <si>
-    <t>NFDI4PSO:0000060</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NFDI4PSO_0000060</t>
-  </si>
-  <si>
     <t>OBI:0001948</t>
   </si>
   <si>
@@ -454,18 +343,6 @@
     <t>http://purl.obolibrary.org/obo/OBI_0001939</t>
   </si>
   <si>
-    <t>NFDI4PSO:0000061</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NFDI4PSO_0000061</t>
-  </si>
-  <si>
-    <t>NFDI4PSO:0000026</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NFDI4PSO_0000026</t>
-  </si>
-  <si>
     <t>Parameter [Processed data file name]</t>
   </si>
   <si>
@@ -473,12 +350,6 @@
   </si>
   <si>
     <t>http://purl.obolibrary.org/obo/NFDI4PSO_0000028</t>
-  </si>
-  <si>
-    <t>NFDI4PSO:0000027</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NFDI4PSO_0000027</t>
   </si>
   <si>
     <t>sample_name</t>
@@ -553,12 +424,6 @@
     <t>Illumina Genome Analyzer IIx</t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/NFDI4PSO_1000038</t>
-  </si>
-  <si>
-    <t>1.1.6</t>
-  </si>
-  <si>
     <t>DataPLANT</t>
   </si>
   <si>
@@ -575,13 +440,154 @@
   </si>
   <si>
     <t>Derived Data File</t>
+  </si>
+  <si>
+    <t>1.1.7</t>
+  </si>
+  <si>
+    <t>Term Source REF (NCIT:C175889)</t>
+  </si>
+  <si>
+    <t>Term Accession Number (NCIT:C175889)</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C175889</t>
+  </si>
+  <si>
+    <t>NCIT</t>
+  </si>
+  <si>
+    <t>NCIT:C175889</t>
+  </si>
+  <si>
+    <t>Parameter [data filtering software]</t>
+  </si>
+  <si>
+    <t>Term Source REF (DPBO:0000023)</t>
+  </si>
+  <si>
+    <t>Term Accession Number (DPBO:0000023)</t>
+  </si>
+  <si>
+    <t>Parameter [data filtering software version]</t>
+  </si>
+  <si>
+    <t>Term Source REF (DPBO:0000024)</t>
+  </si>
+  <si>
+    <t>Term Accession Number (DPBO:0000024)</t>
+  </si>
+  <si>
+    <t>Parameter [data filtering software parameters]</t>
+  </si>
+  <si>
+    <t>Term Source REF (DPBO:0000025)</t>
+  </si>
+  <si>
+    <t>Term Accession Number (DPBO:0000025)</t>
+  </si>
+  <si>
+    <t>Parameter [next generation sequencing instrument model]</t>
+  </si>
+  <si>
+    <t>Term Source REF (DPBO:0000040)</t>
+  </si>
+  <si>
+    <t>Term Accession Number (DPBO:0000040)</t>
+  </si>
+  <si>
+    <t>Parameter [sequence assembly algorithm version]</t>
+  </si>
+  <si>
+    <t>Term Source REF (DPBO:0000060)</t>
+  </si>
+  <si>
+    <t>Term Accession Number (DPBO:0000060)</t>
+  </si>
+  <si>
+    <t>Parameter [genome status]</t>
+  </si>
+  <si>
+    <t>Term Source REF (DPBO:0000061)</t>
+  </si>
+  <si>
+    <t>Term Accession Number (DPBO:0000061)</t>
+  </si>
+  <si>
+    <t>Parameter [genome reference sequence]</t>
+  </si>
+  <si>
+    <t>Term Source REF (DPBO:0000026)</t>
+  </si>
+  <si>
+    <t>Term Accession Number (DPBO:0000026)</t>
+  </si>
+  <si>
+    <t>Parameter [processed data file format]</t>
+  </si>
+  <si>
+    <t>Term Source REF (DPBO:0000027)</t>
+  </si>
+  <si>
+    <t>Term Accession Number (DPBO:0000027)</t>
+  </si>
+  <si>
+    <t>DPBO</t>
+  </si>
+  <si>
+    <t>DPBO:0000027</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/DPBO_0000027</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/DPBO_0000026</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/DPBO_0000061</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/DPBO_0000060</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/DPBO_0000040</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/DPBO_0000025</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/DPBO_0000024</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/DPBO_0000023</t>
+  </si>
+  <si>
+    <t>DPBO:0000023</t>
+  </si>
+  <si>
+    <t>DPBO:0000024</t>
+  </si>
+  <si>
+    <t>DPBO:0000025</t>
+  </si>
+  <si>
+    <t>DPBO:0000040</t>
+  </si>
+  <si>
+    <t>DPBO:0000060</t>
+  </si>
+  <si>
+    <t>DPBO:0000061</t>
+  </si>
+  <si>
+    <t>DPBO:0000026</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -593,6 +599,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFF5F5F5"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -724,10 +738,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -766,11 +781,114 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="34">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
@@ -799,43 +917,43 @@
   <autoFilter ref="A1:AL2" xr:uid="{6313D494-B4F8-4CFB-A5DD-243F71ED2981}"/>
   <tableColumns count="38">
     <tableColumn id="1" xr3:uid="{177A9294-F387-4CC1-A1BB-208B3EDA57DD}" name="Source Name"/>
-    <tableColumn id="3" xr3:uid="{C1843A29-91D2-42FA-BC39-08F9F06EF723}" name="Parameter [BioSample Accession Number]"/>
-    <tableColumn id="4" xr3:uid="{C482A950-68AF-47DD-9595-66378EC25C0A}" name="Term Source REF (NFDI4PSO:0000078)"/>
-    <tableColumn id="5" xr3:uid="{4046016B-3BF0-492F-8EC3-52EB373DDFD4}" name="Term Accession Number (NFDI4PSO:0000078)"/>
-    <tableColumn id="6" xr3:uid="{0BB2A244-AF1D-4954-A3C1-101EE7D571BD}" name="Parameter [Data filtering software]"/>
-    <tableColumn id="7" xr3:uid="{EEF3AFA9-D333-4B6D-A154-8DE976756F50}" name="Term Source REF (NFDI4PSO:0000023)"/>
-    <tableColumn id="8" xr3:uid="{B8D8176E-3A60-4E32-A930-99628C7A2773}" name="Term Accession Number (NFDI4PSO:0000023)"/>
-    <tableColumn id="9" xr3:uid="{AC813E19-4B03-4C73-983C-9D22E46E501C}" name="Parameter [Data filtering software version]"/>
-    <tableColumn id="10" xr3:uid="{48D2D48A-7A67-4CD8-B3AC-E82F068A3A16}" name="Term Source REF (NFDI4PSO:0000024)"/>
-    <tableColumn id="11" xr3:uid="{22F84F4D-1452-43D0-BA92-01A8D5BACD12}" name="Term Accession Number (NFDI4PSO:0000024)"/>
-    <tableColumn id="12" xr3:uid="{C84767BF-DC7D-4374-A054-2509DF4C1408}" name="Parameter [Data filtering Software Parameters]"/>
-    <tableColumn id="13" xr3:uid="{DBFFC409-87BA-4E49-A443-B10EA4A36E85}" name="Term Source REF (NFDI4PSO:0000025)"/>
-    <tableColumn id="14" xr3:uid="{6BC093CF-9E5B-49A7-9216-BE1010FDADC8}" name="Term Accession Number (NFDI4PSO:0000025)"/>
-    <tableColumn id="15" xr3:uid="{82AC7639-98C9-4A5F-A664-415D457A01FA}" name="Parameter [Next generation sequencing instrument model]"/>
-    <tableColumn id="16" xr3:uid="{18DB657D-55F3-4F07-BB99-3F16EB6BAC04}" name="Term Source REF (NFDI4PSO:0000040)"/>
-    <tableColumn id="17" xr3:uid="{9628B434-24C9-47F0-A21D-1A9E82799B25}" name="Term Accession Number (NFDI4PSO:0000040)"/>
+    <tableColumn id="3" xr3:uid="{FBF90856-8880-47F2-AC80-FDEC12D0A866}" name="Parameter [BioSample Accession Number]" dataDxfId="32"/>
+    <tableColumn id="4" xr3:uid="{7CB1F9C4-00BC-4E49-A573-85BFF3059E06}" name="Term Source REF (NCIT:C175889)" dataDxfId="31"/>
+    <tableColumn id="5" xr3:uid="{4AA0CB52-F1AD-4622-9CC7-3E8CAEE3592D}" name="Term Accession Number (NCIT:C175889)" dataDxfId="30"/>
+    <tableColumn id="6" xr3:uid="{1401BD05-0D7D-4533-A957-438E375CD686}" name="Parameter [data filtering software]" dataDxfId="29"/>
+    <tableColumn id="7" xr3:uid="{9C1BF716-D0CA-4E83-9570-9CA40B9D6B64}" name="Term Source REF (DPBO:0000023)" dataDxfId="28"/>
+    <tableColumn id="8" xr3:uid="{35ECBD22-0514-40AA-AFED-B71E54BDAFAC}" name="Term Accession Number (DPBO:0000023)" dataDxfId="27"/>
+    <tableColumn id="9" xr3:uid="{42A2B7F9-85FD-402D-AE8B-EA4BAB2F023C}" name="Parameter [data filtering software version]" dataDxfId="26"/>
+    <tableColumn id="10" xr3:uid="{C65CA552-B5FB-4665-8566-E95ABBE8D0C9}" name="Term Source REF (DPBO:0000024)" dataDxfId="25"/>
+    <tableColumn id="11" xr3:uid="{82AEF731-1688-495F-8F76-6C2A7825596F}" name="Term Accession Number (DPBO:0000024)" dataDxfId="24"/>
+    <tableColumn id="12" xr3:uid="{7C3068A2-C80F-4A87-A0A3-72C4BCE5B60C}" name="Parameter [data filtering software parameters]" dataDxfId="23"/>
+    <tableColumn id="13" xr3:uid="{0CEA6D74-9C94-4322-9786-BE66F0592BE4}" name="Term Source REF (DPBO:0000025)" dataDxfId="22"/>
+    <tableColumn id="14" xr3:uid="{9E9656F2-612F-405C-9AE5-E6C81CF4A526}" name="Term Accession Number (DPBO:0000025)" dataDxfId="21"/>
+    <tableColumn id="15" xr3:uid="{ED0D85B9-D6B1-4B21-A197-24E5AC13C952}" name="Parameter [next generation sequencing instrument model]" dataDxfId="20"/>
+    <tableColumn id="16" xr3:uid="{559E297E-C617-440F-B26C-B46812AC6506}" name="Term Source REF (DPBO:0000040)" dataDxfId="19"/>
+    <tableColumn id="17" xr3:uid="{E820B146-A001-421D-9CE6-368BF3010733}" name="Term Accession Number (DPBO:0000040)" dataDxfId="18"/>
     <tableColumn id="18" xr3:uid="{508D3864-D147-4361-9710-973C9358CB37}" name="Parameter [sequence assembly algorithm]"/>
     <tableColumn id="19" xr3:uid="{8101D462-A442-48DD-9048-D7674381E6CC}" name="Term Source REF (OBI:0001522)"/>
     <tableColumn id="20" xr3:uid="{503FB070-F20C-4BB9-B21E-951423F2C74A}" name="Term Accession Number (OBI:0001522)"/>
-    <tableColumn id="21" xr3:uid="{58E12648-335D-4734-AB72-CF2F66AF9FED}" name="Parameter [Sequence assembly algorithm version]"/>
-    <tableColumn id="22" xr3:uid="{8659A64E-47AC-48D3-ABCD-2DA57ECB06FB}" name="Term Source REF (NFDI4PSO:0000060)"/>
-    <tableColumn id="23" xr3:uid="{C347A7B1-32FF-4EC4-A3C2-7CD32321B7C2}" name="Term Accession Number (NFDI4PSO:0000060)"/>
-    <tableColumn id="24" xr3:uid="{0B9D146C-24DE-44DF-AD5C-240784D0148E}" name="Parameter [sequence assembly name]"/>
-    <tableColumn id="25" xr3:uid="{436726B1-D092-4392-8056-799BCFA07BE0}" name="Term Source REF (OBI:0001948)"/>
-    <tableColumn id="26" xr3:uid="{2A11ADD0-9BFF-4FA3-B714-AC7B9F777C2E}" name="Term Accession Number (OBI:0001948)"/>
-    <tableColumn id="27" xr3:uid="{E9F38BD7-6598-4BFE-B4C1-0F5B5C219304}" name="Parameter [genome coverage]"/>
-    <tableColumn id="28" xr3:uid="{0912FD02-522C-4409-B9E2-B489B359B30E}" name="Term Source REF (OBI:0001939)"/>
-    <tableColumn id="29" xr3:uid="{506A0FCA-0FB2-4FB2-9975-6836C867BA6B}" name="Term Accession Number (OBI:0001939)"/>
-    <tableColumn id="30" xr3:uid="{AE623F81-44BA-46A3-8A5C-ACE0868DDFA7}" name="Parameter [Genome status]"/>
-    <tableColumn id="31" xr3:uid="{3320AC11-BA81-4298-995B-7EC96A12F53F}" name="Term Source REF (NFDI4PSO:0000061)"/>
-    <tableColumn id="32" xr3:uid="{FF2E1974-5E0F-42E7-9002-46EB5B766917}" name="Term Accession Number (NFDI4PSO:0000061)"/>
-    <tableColumn id="33" xr3:uid="{67D4BA13-CFE2-4E7F-BE4B-1E9517629FA2}" name="Parameter [Genome reference sequence]"/>
-    <tableColumn id="34" xr3:uid="{E6DB6F73-C437-461C-95D5-72089D1BBC91}" name="Term Source REF (NFDI4PSO:0000026)"/>
-    <tableColumn id="35" xr3:uid="{64963BB5-8C8C-4A03-955B-1062169C3FA1}" name="Term Accession Number (NFDI4PSO:0000026)"/>
-    <tableColumn id="36" xr3:uid="{BABEB0E1-C070-4A62-BA72-FDA195146EFD}" name="Parameter [Processed data file format]"/>
-    <tableColumn id="37" xr3:uid="{8611E0EA-5557-4A72-9D69-AAF4C5BBCA3F}" name="Term Source REF (NFDI4PSO:0000027)"/>
-    <tableColumn id="38" xr3:uid="{77A26896-8666-47F3-8757-1DBF8D855FA0}" name="Term Accession Number (NFDI4PSO:0000027)"/>
-    <tableColumn id="2" xr3:uid="{37AAA820-E44D-492C-A2D8-56248E8B1009}" name="Derived Data File" dataDxfId="0"/>
+    <tableColumn id="21" xr3:uid="{2A2CE47F-1923-4069-B483-4A0A86ECC874}" name="Parameter [sequence assembly algorithm version]" dataDxfId="17"/>
+    <tableColumn id="22" xr3:uid="{EABEA025-9DE7-418D-A198-706E3559D894}" name="Term Source REF (DPBO:0000060)" dataDxfId="16"/>
+    <tableColumn id="23" xr3:uid="{D3ECB70E-91D6-4FD2-9C4F-F9E7AF9B4B4B}" name="Term Accession Number (DPBO:0000060)" dataDxfId="15"/>
+    <tableColumn id="40" xr3:uid="{46670F83-9D63-48AD-98A3-8E197E1CC306}" name="Parameter [sequence assembly name]" dataDxfId="14"/>
+    <tableColumn id="41" xr3:uid="{C703A56D-03B1-4755-A660-37B4174E1F0D}" name="Term Source REF (OBI:0001948)" dataDxfId="13"/>
+    <tableColumn id="42" xr3:uid="{EAF18FF4-C9E4-4F34-A3F3-DDD9F0E64A1E}" name="Term Accession Number (OBI:0001948)" dataDxfId="12"/>
+    <tableColumn id="43" xr3:uid="{66EEE367-EFA6-4812-A7A7-BE4886A6824D}" name="Parameter [genome coverage]" dataDxfId="11"/>
+    <tableColumn id="44" xr3:uid="{010F232B-5FCE-4463-81B6-C091A58C4651}" name="Term Source REF (OBI:0001939)" dataDxfId="10"/>
+    <tableColumn id="45" xr3:uid="{C0CAB42F-A92F-4D37-A333-8E83816145B2}" name="Term Accession Number (OBI:0001939)" dataDxfId="9"/>
+    <tableColumn id="46" xr3:uid="{B284403A-6425-4F12-92AD-BF927CA6CE08}" name="Parameter [genome status]" dataDxfId="8"/>
+    <tableColumn id="47" xr3:uid="{E0FF587D-3D23-4C0B-AC12-91911D067572}" name="Term Source REF (DPBO:0000061)" dataDxfId="7"/>
+    <tableColumn id="48" xr3:uid="{77077C0E-6C5B-461E-B8B4-F8EFC42935B8}" name="Term Accession Number (DPBO:0000061)" dataDxfId="6"/>
+    <tableColumn id="49" xr3:uid="{00ECFF3A-1744-44CB-9ADF-2CC0FF569074}" name="Parameter [genome reference sequence]" dataDxfId="5"/>
+    <tableColumn id="50" xr3:uid="{925FA146-4B22-4022-9B72-F9581FE927ED}" name="Term Source REF (DPBO:0000026)" dataDxfId="4"/>
+    <tableColumn id="51" xr3:uid="{08E8013B-595D-4457-8617-D5F7FF7762DD}" name="Term Accession Number (DPBO:0000026)" dataDxfId="3"/>
+    <tableColumn id="52" xr3:uid="{BF863F98-6FFC-4BFA-835F-A6B908BB2D7F}" name="Parameter [processed data file format]" dataDxfId="2"/>
+    <tableColumn id="53" xr3:uid="{D3248941-950E-49FD-AC3A-6C840CBC005D}" name="Term Source REF (DPBO:0000027)" dataDxfId="1"/>
+    <tableColumn id="54" xr3:uid="{10615F06-CF59-4F32-A281-0BD2B35F19E0}" name="Term Accession Number (DPBO:0000027)" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{37AAA820-E44D-492C-A2D8-56248E8B1009}" name="Derived Data File" dataDxfId="33"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1139,7 +1257,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="350" row="3">
+  <wetp:taskpane dockstate="right" visibility="0" width="680" row="0">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
   <wetp:taskpane dockstate="right" visibility="0" width="656" row="2">
@@ -1172,53 +1290,53 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AL2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
-      <selection activeCell="AI2" sqref="AI2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AF21" sqref="AF21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.7109375" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="35" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="36.7109375" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="42.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="36.7109375" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="46.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="36.7109375" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="57.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="36.7109375" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="46.5703125" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="41.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="30.85546875" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="37.85546875" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="49.140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="36.7109375" hidden="1" customWidth="1"/>
-    <col min="22" max="22" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="23" max="23" width="38" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="30.85546875" hidden="1" customWidth="1"/>
-    <col min="25" max="25" width="37.85546875" hidden="1" customWidth="1"/>
-    <col min="26" max="26" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="30.85546875" hidden="1" customWidth="1"/>
-    <col min="28" max="28" width="37.85546875" hidden="1" customWidth="1"/>
-    <col min="29" max="29" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="36.7109375" hidden="1" customWidth="1"/>
-    <col min="31" max="31" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="32" max="32" width="41.28515625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="36.7109375" hidden="1" customWidth="1"/>
-    <col min="34" max="34" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="35" max="35" width="38.42578125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="36.7109375" hidden="1" customWidth="1"/>
-    <col min="37" max="37" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="38" max="38" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="37.44140625" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="32.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.6640625" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="38.109375" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="39.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31.6640625" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="38.109375" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="42.77734375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="31.6640625" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="38.109375" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="53.21875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="31.6640625" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="38.109375" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="39.109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="29.88671875" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="36.33203125" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="45.77734375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="31.6640625" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="38.109375" hidden="1" customWidth="1"/>
+    <col min="23" max="23" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="29.88671875" hidden="1" customWidth="1"/>
+    <col min="25" max="25" width="36.33203125" hidden="1" customWidth="1"/>
+    <col min="26" max="26" width="29.109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="29.88671875" hidden="1" customWidth="1"/>
+    <col min="28" max="28" width="36.33203125" hidden="1" customWidth="1"/>
+    <col min="29" max="29" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="31.6640625" hidden="1" customWidth="1"/>
+    <col min="31" max="31" width="38.109375" hidden="1" customWidth="1"/>
+    <col min="32" max="32" width="38" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="31.6640625" hidden="1" customWidth="1"/>
+    <col min="34" max="34" width="38.109375" hidden="1" customWidth="1"/>
+    <col min="35" max="35" width="36.109375" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="31.6640625" hidden="1" customWidth="1"/>
+    <col min="37" max="37" width="38.109375" hidden="1" customWidth="1"/>
+    <col min="38" max="38" width="17.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1226,123 +1344,209 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G1" t="s">
+        <v>111</v>
+      </c>
+      <c r="H1" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1" t="s">
+        <v>113</v>
+      </c>
+      <c r="J1" t="s">
+        <v>114</v>
+      </c>
+      <c r="K1" t="s">
+        <v>115</v>
+      </c>
+      <c r="L1" t="s">
+        <v>116</v>
+      </c>
+      <c r="M1" t="s">
+        <v>117</v>
+      </c>
+      <c r="N1" t="s">
+        <v>118</v>
+      </c>
+      <c r="O1" t="s">
+        <v>119</v>
+      </c>
+      <c r="P1" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="R1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="S1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="T1" t="s">
+        <v>121</v>
+      </c>
+      <c r="U1" t="s">
+        <v>122</v>
+      </c>
+      <c r="V1" t="s">
+        <v>123</v>
+      </c>
+      <c r="W1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="X1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="Y1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="Z1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="AA1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="AB1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" t="s">
-        <v>21</v>
-      </c>
-      <c r="W1" t="s">
-        <v>22</v>
-      </c>
-      <c r="X1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>27</v>
-      </c>
       <c r="AC1" t="s">
-        <v>28</v>
+        <v>124</v>
       </c>
       <c r="AD1" t="s">
-        <v>29</v>
+        <v>125</v>
       </c>
       <c r="AE1" t="s">
-        <v>30</v>
+        <v>126</v>
       </c>
       <c r="AF1" t="s">
-        <v>31</v>
+        <v>127</v>
       </c>
       <c r="AG1" t="s">
-        <v>32</v>
+        <v>128</v>
       </c>
       <c r="AH1" t="s">
-        <v>33</v>
+        <v>129</v>
       </c>
       <c r="AI1" t="s">
-        <v>34</v>
+        <v>130</v>
       </c>
       <c r="AJ1" t="s">
-        <v>35</v>
+        <v>131</v>
       </c>
       <c r="AK1" t="s">
-        <v>36</v>
+        <v>132</v>
       </c>
       <c r="AL1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="B2" s="13"/>
+      <c r="C2" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="J2" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="K2" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="L2" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="M2" s="13" t="s">
+        <v>50</v>
+      </c>
       <c r="N2" t="s">
-        <v>139</v>
-      </c>
-      <c r="O2" t="s">
-        <v>89</v>
-      </c>
-      <c r="P2" t="s">
-        <v>140</v>
+        <v>96</v>
+      </c>
+      <c r="O2" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="P2" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="T2" s="13"/>
+      <c r="U2" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="V2" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="W2" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="X2" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y2" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="Z2" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA2" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="AB2" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="AC2" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="AD2" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="AE2" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="AF2" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="AG2" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="AH2" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="AI2" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="AJ2" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="AK2" s="13" t="s">
+        <v>50</v>
       </c>
       <c r="AL2" s="13"/>
     </row>
@@ -1359,248 +1563,248 @@
   <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="57.140625" customWidth="1"/>
+    <col min="1" max="1" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="57.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>43</v>
+        <v>18</v>
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>44</v>
+        <v>19</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>64</v>
+        <v>39</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="D8" s="8"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>46</v>
+        <v>21</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>48</v>
+        <v>23</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>66</v>
+        <v>41</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>67</v>
+        <v>42</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>49</v>
+        <v>24</v>
       </c>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>51</v>
+        <v>26</v>
       </c>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>69</v>
+        <v>44</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>70</v>
+        <v>45</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>53</v>
+        <v>28</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>72</v>
+        <v>47</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>73</v>
+        <v>48</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>55</v>
+        <v>30</v>
       </c>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>57</v>
+        <v>32</v>
       </c>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>58</v>
+        <v>33</v>
       </c>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>59</v>
+        <v>34</v>
       </c>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>143</v>
+        <v>98</v>
       </c>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>144</v>
+        <v>99</v>
       </c>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>145</v>
+        <v>100</v>
       </c>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
-        <v>146</v>
+        <v>101</v>
       </c>
       <c r="B27" s="9"/>
       <c r="C27" s="9"/>
@@ -1616,80 +1820,82 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="54.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="46.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="54.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>76</v>
+        <v>51</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>77</v>
+        <v>52</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>78</v>
+        <v>53</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>79</v>
+        <v>54</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>80</v>
+        <v>55</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>81</v>
+        <v>56</v>
       </c>
       <c r="H1" s="11" t="s">
-        <v>82</v>
+        <v>57</v>
       </c>
       <c r="I1" s="11" t="s">
-        <v>83</v>
+        <v>58</v>
       </c>
       <c r="J1" s="11" t="s">
-        <v>84</v>
+        <v>59</v>
       </c>
       <c r="K1" s="11" t="s">
-        <v>85</v>
+        <v>60</v>
       </c>
       <c r="L1" s="11" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
@@ -1698,332 +1904,332 @@
       <c r="K2" s="12"/>
       <c r="L2" s="12"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
-        <v>87</v>
+        <v>62</v>
       </c>
       <c r="B3" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="H3" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="C3" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="G3" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="H3" s="12" t="s">
-        <v>118</v>
-      </c>
       <c r="I3" s="12" t="s">
-        <v>119</v>
+        <v>76</v>
       </c>
       <c r="J3" s="12"/>
       <c r="K3" s="12"/>
       <c r="L3" s="12"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>88</v>
+        <v>108</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>90</v>
+        <v>107</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>106</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>120</v>
+        <v>77</v>
       </c>
       <c r="H4" s="12" t="s">
-        <v>121</v>
+        <v>78</v>
       </c>
       <c r="I4" s="12" t="s">
-        <v>119</v>
+        <v>76</v>
       </c>
       <c r="J4" s="12"/>
       <c r="K4" s="12"/>
       <c r="L4" s="12"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
-        <v>4</v>
+        <v>109</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>91</v>
+        <v>143</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>92</v>
+        <v>133</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>142</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
       <c r="I5" s="12" t="s">
-        <v>122</v>
+        <v>79</v>
       </c>
       <c r="J5" s="12"/>
       <c r="K5" s="12"/>
       <c r="L5" s="12"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
-        <v>7</v>
+        <v>112</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>93</v>
+        <v>144</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>94</v>
+        <v>133</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>141</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="G6" s="12"/>
       <c r="H6" s="12"/>
       <c r="I6" s="12" t="s">
-        <v>122</v>
+        <v>79</v>
       </c>
       <c r="J6" s="12"/>
       <c r="K6" s="12"/>
       <c r="L6" s="12"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
-        <v>10</v>
+        <v>115</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>95</v>
+        <v>145</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>96</v>
+        <v>133</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>140</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="G7" s="12"/>
       <c r="H7" s="12"/>
       <c r="I7" s="12" t="s">
-        <v>122</v>
+        <v>79</v>
       </c>
       <c r="J7" s="12"/>
       <c r="K7" s="12"/>
       <c r="L7" s="12"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
-        <v>13</v>
+        <v>118</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>97</v>
+        <v>146</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>98</v>
+        <v>133</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>139</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>123</v>
+        <v>80</v>
       </c>
       <c r="H8" s="12" t="s">
-        <v>124</v>
+        <v>81</v>
       </c>
       <c r="I8" s="12" t="s">
-        <v>125</v>
+        <v>82</v>
       </c>
       <c r="J8" s="12"/>
       <c r="K8" s="12"/>
       <c r="L8" s="12"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>99</v>
+        <v>64</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>100</v>
+        <v>65</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>101</v>
+        <v>66</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>126</v>
+        <v>83</v>
       </c>
       <c r="H9" s="12" t="s">
-        <v>127</v>
+        <v>84</v>
       </c>
       <c r="I9" s="12" t="s">
-        <v>125</v>
+        <v>82</v>
       </c>
       <c r="J9" s="12"/>
       <c r="K9" s="12"/>
       <c r="L9" s="12"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
-        <v>19</v>
+        <v>121</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>102</v>
+        <v>147</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>103</v>
+        <v>133</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>138</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>128</v>
+        <v>85</v>
       </c>
       <c r="H10" s="12" t="s">
-        <v>129</v>
+        <v>86</v>
       </c>
       <c r="I10" s="12" t="s">
-        <v>119</v>
+        <v>76</v>
       </c>
       <c r="J10" s="12"/>
       <c r="K10" s="12"/>
       <c r="L10" s="12"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="11" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>104</v>
+        <v>67</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>100</v>
+        <v>65</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>105</v>
+        <v>68</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>130</v>
+        <v>87</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>131</v>
+        <v>88</v>
       </c>
       <c r="I11" s="12" t="s">
-        <v>132</v>
+        <v>89</v>
       </c>
       <c r="J11" s="12"/>
       <c r="K11" s="12"/>
       <c r="L11" s="12"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="11" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>106</v>
+        <v>69</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>100</v>
+        <v>65</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>107</v>
+        <v>70</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>133</v>
+        <v>90</v>
       </c>
       <c r="H12" s="12" t="s">
-        <v>134</v>
+        <v>91</v>
       </c>
       <c r="I12" s="12" t="s">
-        <v>119</v>
+        <v>76</v>
       </c>
       <c r="J12" s="12"/>
       <c r="K12" s="12"/>
       <c r="L12" s="12"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
-        <v>28</v>
+        <v>124</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>108</v>
+        <v>148</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="D13" s="12" t="s">
-        <v>109</v>
+        <v>133</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>137</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="G13" s="12"/>
       <c r="H13" s="12"/>
@@ -2032,99 +2238,111 @@
       <c r="K13" s="12"/>
       <c r="L13" s="12"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
-        <v>31</v>
+        <v>127</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>110</v>
+        <v>149</v>
       </c>
       <c r="C14" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="H14" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="I14" s="12" t="s">
         <v>89</v>
-      </c>
-      <c r="D14" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="E14" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="F14" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="G14" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="H14" s="12" t="s">
-        <v>136</v>
-      </c>
-      <c r="I14" s="12" t="s">
-        <v>132</v>
       </c>
       <c r="J14" s="12"/>
       <c r="K14" s="12"/>
       <c r="L14" s="12"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="11" t="s">
-        <v>112</v>
+        <v>71</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>113</v>
+        <v>72</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="D15" s="12" t="s">
-        <v>114</v>
+        <v>63</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>73</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>137</v>
+        <v>94</v>
       </c>
       <c r="H15" s="12" t="s">
-        <v>138</v>
+        <v>95</v>
       </c>
       <c r="I15" s="12" t="s">
-        <v>119</v>
+        <v>76</v>
       </c>
       <c r="J15" s="12"/>
       <c r="K15" s="12"/>
       <c r="L15" s="12"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>115</v>
+        <v>134</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="D16" s="12" t="s">
-        <v>116</v>
+        <v>133</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>135</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="G16" s="12"/>
       <c r="H16" s="12"/>
       <c r="I16" s="12" t="s">
-        <v>122</v>
+        <v>79</v>
       </c>
       <c r="J16" s="12"/>
       <c r="K16" s="12"/>
       <c r="L16" s="12"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D4" r:id="rId1" xr:uid="{70751FB4-3F9A-459E-B046-9B0EECB4A0D8}"/>
+    <hyperlink ref="D15" r:id="rId2" xr:uid="{80587771-CC40-449D-A1D0-49C75D9E77D2}"/>
+    <hyperlink ref="D16" r:id="rId3" xr:uid="{8A285B46-9EA4-4698-B24B-C2B5B2EA1D80}"/>
+    <hyperlink ref="D14" r:id="rId4" xr:uid="{5790CB73-E2F2-445A-BC68-57C899A1A781}"/>
+    <hyperlink ref="D13" r:id="rId5" xr:uid="{3AA6D27E-3C0E-45AD-A5E9-A38E62A0C056}"/>
+    <hyperlink ref="D10" r:id="rId6" xr:uid="{9BF6325D-AC6A-4718-A9F4-5881E7249E90}"/>
+    <hyperlink ref="D8" r:id="rId7" xr:uid="{E590CA81-5DF1-4B93-B5BD-8505F334733D}"/>
+    <hyperlink ref="D7" r:id="rId8" xr:uid="{5A370DF3-F3F8-4802-9881-54DC222DE7A9}"/>
+    <hyperlink ref="D6" r:id="rId9" xr:uid="{92D423C2-EA43-4B2C-873E-695C1FE4368A}"/>
+    <hyperlink ref="D5" r:id="rId10" xr:uid="{B2A3C0E0-5969-4820-B230-D2C4226802A6}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
exchanged term from genbank "mapping"
</commit_message>
<xml_diff>
--- a/templates/dataplant/4COM04_GenomeAssembly.xlsx
+++ b/templates/dataplant/4COM04_GenomeAssembly.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stella Eggels\sciebo - Eggels, Stella (s.eggels@fz-juelich.de)@fz-juelich.sciebo.de\SE\DataPLANT\ARCs und SWATE\ersatz von nfdi4pso\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dominikbrilhaus/github/nfdi4plants/Swate-templates/templates/dataplant/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{828227F5-40BA-4FC4-9040-C62E6D82AD2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{475A4500-2A89-0E47-B12E-EF4E317DAB69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1900" yWindow="500" windowWidth="27860" windowHeight="17500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="4COM04_GenomeAssembly" sheetId="1" r:id="rId1"/>
@@ -51,76 +51,157 @@
   <commentList>
     <comment ref="A1" authorId="0" shapeId="0" xr:uid="{1B82A122-B7DC-4A5B-92B7-EFF54693A4C6}">
       <text>
-        <t>[Kommentarthread]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
 Kommentar:
     The unique identifier of this template. It will be auto generated.
 Antwort:
     id=11b23480-80a8-4d95-a2bb-b3e9c7d53a23</t>
+        </r>
       </text>
     </comment>
     <comment ref="A2" authorId="1" shapeId="0" xr:uid="{7F2B0E6D-7667-4BBE-84EF-E94F714AF9D5}">
       <text>
-        <t>[Kommentarthread]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
 Kommentar:
     The name of the Swate template.</t>
+        </r>
       </text>
     </comment>
     <comment ref="A3" authorId="2" shapeId="0" xr:uid="{55280B2E-9540-497C-8359-55487A5C5B18}">
       <text>
-        <t>[Kommentarthread]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
 Kommentar:
     The current version of this template in SemVer notation.</t>
+        </r>
       </text>
     </comment>
     <comment ref="A4" authorId="3" shapeId="0" xr:uid="{F0D435E2-551F-45A7-BCE6-994AC7ADA3CA}">
       <text>
-        <t>[Kommentarthread]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
 Kommentar:
     The description of this template. Use few sentences for succinctness.</t>
+        </r>
       </text>
     </comment>
     <comment ref="A5" authorId="4" shapeId="0" xr:uid="{E6BCAC0A-6199-4E14-8166-0207D5BB43BA}">
       <text>
-        <t>[Kommentarthread]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
 Kommentar:
     The name of the template associated organisation. "DataPLANT" will trigger the "DataPLANT" batch of honor for the template.</t>
+        </r>
       </text>
     </comment>
     <comment ref="A6" authorId="5" shapeId="0" xr:uid="{60BEB3E6-604B-45C4-BB34-C8023C7A5426}">
       <text>
-        <t>[Kommentarthread]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
 Kommentar:
     The name of the Swate annotation table in the workbook of the template's excel file.</t>
+        </r>
       </text>
     </comment>
     <comment ref="A7" authorId="6" shapeId="0" xr:uid="{3F4F0D99-C656-496E-AC9C-D9F60E63A964}">
       <text>
-        <t>[Kommentarthread]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
 Kommentar:
     A list of all ERs (endpoint repositories) targeted with this template. ERs are realized as Terms: &lt;term ref here&gt;</t>
+        </r>
       </text>
     </comment>
     <comment ref="A11" authorId="7" shapeId="0" xr:uid="{9FE4B02B-3403-489E-8E1F-763CB8E6BEEA}">
       <text>
-        <t>[Kommentarthread]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
 Kommentar:
     A list of all tags associated with this template. Tags are realized as Terms: &lt;term ref here&gt;</t>
+        </r>
       </text>
     </comment>
     <comment ref="A15" authorId="8" shapeId="0" xr:uid="{CDC4E02C-8CF8-4363-A689-0DE050A2C5DC}">
       <text>
-        <t>[Kommentarthread]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
 Kommentar:
     The author(s) of this template.</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -128,7 +209,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="146">
   <si>
     <t>Source Name</t>
   </si>
@@ -319,9 +400,6 @@
     <t>Sample Name</t>
   </si>
   <si>
-    <t>NFDI4PSO</t>
-  </si>
-  <si>
     <t>OBI:0001522</t>
   </si>
   <si>
@@ -341,15 +419,6 @@
   </si>
   <si>
     <t>http://purl.obolibrary.org/obo/OBI_0001939</t>
-  </si>
-  <si>
-    <t>Parameter [Processed data file name]</t>
-  </si>
-  <si>
-    <t>NFDI4PSO:0000028</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NFDI4PSO_0000028</t>
   </si>
   <si>
     <t>sample_name</t>
@@ -786,8 +855,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Link" xfId="1" builtinId="8"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="34">
     <dxf>
@@ -917,43 +986,43 @@
   <autoFilter ref="A1:AL2" xr:uid="{6313D494-B4F8-4CFB-A5DD-243F71ED2981}"/>
   <tableColumns count="38">
     <tableColumn id="1" xr3:uid="{177A9294-F387-4CC1-A1BB-208B3EDA57DD}" name="Source Name"/>
-    <tableColumn id="3" xr3:uid="{FBF90856-8880-47F2-AC80-FDEC12D0A866}" name="Parameter [BioSample Accession Number]" dataDxfId="32"/>
-    <tableColumn id="4" xr3:uid="{7CB1F9C4-00BC-4E49-A573-85BFF3059E06}" name="Term Source REF (NCIT:C175889)" dataDxfId="31"/>
-    <tableColumn id="5" xr3:uid="{4AA0CB52-F1AD-4622-9CC7-3E8CAEE3592D}" name="Term Accession Number (NCIT:C175889)" dataDxfId="30"/>
-    <tableColumn id="6" xr3:uid="{1401BD05-0D7D-4533-A957-438E375CD686}" name="Parameter [data filtering software]" dataDxfId="29"/>
-    <tableColumn id="7" xr3:uid="{9C1BF716-D0CA-4E83-9570-9CA40B9D6B64}" name="Term Source REF (DPBO:0000023)" dataDxfId="28"/>
-    <tableColumn id="8" xr3:uid="{35ECBD22-0514-40AA-AFED-B71E54BDAFAC}" name="Term Accession Number (DPBO:0000023)" dataDxfId="27"/>
-    <tableColumn id="9" xr3:uid="{42A2B7F9-85FD-402D-AE8B-EA4BAB2F023C}" name="Parameter [data filtering software version]" dataDxfId="26"/>
-    <tableColumn id="10" xr3:uid="{C65CA552-B5FB-4665-8566-E95ABBE8D0C9}" name="Term Source REF (DPBO:0000024)" dataDxfId="25"/>
-    <tableColumn id="11" xr3:uid="{82AEF731-1688-495F-8F76-6C2A7825596F}" name="Term Accession Number (DPBO:0000024)" dataDxfId="24"/>
-    <tableColumn id="12" xr3:uid="{7C3068A2-C80F-4A87-A0A3-72C4BCE5B60C}" name="Parameter [data filtering software parameters]" dataDxfId="23"/>
-    <tableColumn id="13" xr3:uid="{0CEA6D74-9C94-4322-9786-BE66F0592BE4}" name="Term Source REF (DPBO:0000025)" dataDxfId="22"/>
-    <tableColumn id="14" xr3:uid="{9E9656F2-612F-405C-9AE5-E6C81CF4A526}" name="Term Accession Number (DPBO:0000025)" dataDxfId="21"/>
-    <tableColumn id="15" xr3:uid="{ED0D85B9-D6B1-4B21-A197-24E5AC13C952}" name="Parameter [next generation sequencing instrument model]" dataDxfId="20"/>
-    <tableColumn id="16" xr3:uid="{559E297E-C617-440F-B26C-B46812AC6506}" name="Term Source REF (DPBO:0000040)" dataDxfId="19"/>
-    <tableColumn id="17" xr3:uid="{E820B146-A001-421D-9CE6-368BF3010733}" name="Term Accession Number (DPBO:0000040)" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{FBF90856-8880-47F2-AC80-FDEC12D0A866}" name="Parameter [BioSample Accession Number]" dataDxfId="33"/>
+    <tableColumn id="4" xr3:uid="{7CB1F9C4-00BC-4E49-A573-85BFF3059E06}" name="Term Source REF (NCIT:C175889)" dataDxfId="32"/>
+    <tableColumn id="5" xr3:uid="{4AA0CB52-F1AD-4622-9CC7-3E8CAEE3592D}" name="Term Accession Number (NCIT:C175889)" dataDxfId="31"/>
+    <tableColumn id="6" xr3:uid="{1401BD05-0D7D-4533-A957-438E375CD686}" name="Parameter [data filtering software]" dataDxfId="30"/>
+    <tableColumn id="7" xr3:uid="{9C1BF716-D0CA-4E83-9570-9CA40B9D6B64}" name="Term Source REF (DPBO:0000023)" dataDxfId="29"/>
+    <tableColumn id="8" xr3:uid="{35ECBD22-0514-40AA-AFED-B71E54BDAFAC}" name="Term Accession Number (DPBO:0000023)" dataDxfId="28"/>
+    <tableColumn id="9" xr3:uid="{42A2B7F9-85FD-402D-AE8B-EA4BAB2F023C}" name="Parameter [data filtering software version]" dataDxfId="27"/>
+    <tableColumn id="10" xr3:uid="{C65CA552-B5FB-4665-8566-E95ABBE8D0C9}" name="Term Source REF (DPBO:0000024)" dataDxfId="26"/>
+    <tableColumn id="11" xr3:uid="{82AEF731-1688-495F-8F76-6C2A7825596F}" name="Term Accession Number (DPBO:0000024)" dataDxfId="25"/>
+    <tableColumn id="12" xr3:uid="{7C3068A2-C80F-4A87-A0A3-72C4BCE5B60C}" name="Parameter [data filtering software parameters]" dataDxfId="24"/>
+    <tableColumn id="13" xr3:uid="{0CEA6D74-9C94-4322-9786-BE66F0592BE4}" name="Term Source REF (DPBO:0000025)" dataDxfId="23"/>
+    <tableColumn id="14" xr3:uid="{9E9656F2-612F-405C-9AE5-E6C81CF4A526}" name="Term Accession Number (DPBO:0000025)" dataDxfId="22"/>
+    <tableColumn id="15" xr3:uid="{ED0D85B9-D6B1-4B21-A197-24E5AC13C952}" name="Parameter [next generation sequencing instrument model]" dataDxfId="21"/>
+    <tableColumn id="16" xr3:uid="{559E297E-C617-440F-B26C-B46812AC6506}" name="Term Source REF (DPBO:0000040)" dataDxfId="20"/>
+    <tableColumn id="17" xr3:uid="{E820B146-A001-421D-9CE6-368BF3010733}" name="Term Accession Number (DPBO:0000040)" dataDxfId="19"/>
     <tableColumn id="18" xr3:uid="{508D3864-D147-4361-9710-973C9358CB37}" name="Parameter [sequence assembly algorithm]"/>
     <tableColumn id="19" xr3:uid="{8101D462-A442-48DD-9048-D7674381E6CC}" name="Term Source REF (OBI:0001522)"/>
     <tableColumn id="20" xr3:uid="{503FB070-F20C-4BB9-B21E-951423F2C74A}" name="Term Accession Number (OBI:0001522)"/>
-    <tableColumn id="21" xr3:uid="{2A2CE47F-1923-4069-B483-4A0A86ECC874}" name="Parameter [sequence assembly algorithm version]" dataDxfId="17"/>
-    <tableColumn id="22" xr3:uid="{EABEA025-9DE7-418D-A198-706E3559D894}" name="Term Source REF (DPBO:0000060)" dataDxfId="16"/>
-    <tableColumn id="23" xr3:uid="{D3ECB70E-91D6-4FD2-9C4F-F9E7AF9B4B4B}" name="Term Accession Number (DPBO:0000060)" dataDxfId="15"/>
-    <tableColumn id="40" xr3:uid="{46670F83-9D63-48AD-98A3-8E197E1CC306}" name="Parameter [sequence assembly name]" dataDxfId="14"/>
-    <tableColumn id="41" xr3:uid="{C703A56D-03B1-4755-A660-37B4174E1F0D}" name="Term Source REF (OBI:0001948)" dataDxfId="13"/>
-    <tableColumn id="42" xr3:uid="{EAF18FF4-C9E4-4F34-A3F3-DDD9F0E64A1E}" name="Term Accession Number (OBI:0001948)" dataDxfId="12"/>
-    <tableColumn id="43" xr3:uid="{66EEE367-EFA6-4812-A7A7-BE4886A6824D}" name="Parameter [genome coverage]" dataDxfId="11"/>
-    <tableColumn id="44" xr3:uid="{010F232B-5FCE-4463-81B6-C091A58C4651}" name="Term Source REF (OBI:0001939)" dataDxfId="10"/>
-    <tableColumn id="45" xr3:uid="{C0CAB42F-A92F-4D37-A333-8E83816145B2}" name="Term Accession Number (OBI:0001939)" dataDxfId="9"/>
-    <tableColumn id="46" xr3:uid="{B284403A-6425-4F12-92AD-BF927CA6CE08}" name="Parameter [genome status]" dataDxfId="8"/>
-    <tableColumn id="47" xr3:uid="{E0FF587D-3D23-4C0B-AC12-91911D067572}" name="Term Source REF (DPBO:0000061)" dataDxfId="7"/>
-    <tableColumn id="48" xr3:uid="{77077C0E-6C5B-461E-B8B4-F8EFC42935B8}" name="Term Accession Number (DPBO:0000061)" dataDxfId="6"/>
-    <tableColumn id="49" xr3:uid="{00ECFF3A-1744-44CB-9ADF-2CC0FF569074}" name="Parameter [genome reference sequence]" dataDxfId="5"/>
-    <tableColumn id="50" xr3:uid="{925FA146-4B22-4022-9B72-F9581FE927ED}" name="Term Source REF (DPBO:0000026)" dataDxfId="4"/>
-    <tableColumn id="51" xr3:uid="{08E8013B-595D-4457-8617-D5F7FF7762DD}" name="Term Accession Number (DPBO:0000026)" dataDxfId="3"/>
-    <tableColumn id="52" xr3:uid="{BF863F98-6FFC-4BFA-835F-A6B908BB2D7F}" name="Parameter [processed data file format]" dataDxfId="2"/>
-    <tableColumn id="53" xr3:uid="{D3248941-950E-49FD-AC3A-6C840CBC005D}" name="Term Source REF (DPBO:0000027)" dataDxfId="1"/>
-    <tableColumn id="54" xr3:uid="{10615F06-CF59-4F32-A281-0BD2B35F19E0}" name="Term Accession Number (DPBO:0000027)" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{37AAA820-E44D-492C-A2D8-56248E8B1009}" name="Derived Data File" dataDxfId="33"/>
+    <tableColumn id="21" xr3:uid="{2A2CE47F-1923-4069-B483-4A0A86ECC874}" name="Parameter [sequence assembly algorithm version]" dataDxfId="18"/>
+    <tableColumn id="22" xr3:uid="{EABEA025-9DE7-418D-A198-706E3559D894}" name="Term Source REF (DPBO:0000060)" dataDxfId="17"/>
+    <tableColumn id="23" xr3:uid="{D3ECB70E-91D6-4FD2-9C4F-F9E7AF9B4B4B}" name="Term Accession Number (DPBO:0000060)" dataDxfId="16"/>
+    <tableColumn id="40" xr3:uid="{46670F83-9D63-48AD-98A3-8E197E1CC306}" name="Parameter [sequence assembly name]" dataDxfId="15"/>
+    <tableColumn id="41" xr3:uid="{C703A56D-03B1-4755-A660-37B4174E1F0D}" name="Term Source REF (OBI:0001948)" dataDxfId="14"/>
+    <tableColumn id="42" xr3:uid="{EAF18FF4-C9E4-4F34-A3F3-DDD9F0E64A1E}" name="Term Accession Number (OBI:0001948)" dataDxfId="13"/>
+    <tableColumn id="43" xr3:uid="{66EEE367-EFA6-4812-A7A7-BE4886A6824D}" name="Parameter [genome coverage]" dataDxfId="12"/>
+    <tableColumn id="44" xr3:uid="{010F232B-5FCE-4463-81B6-C091A58C4651}" name="Term Source REF (OBI:0001939)" dataDxfId="11"/>
+    <tableColumn id="45" xr3:uid="{C0CAB42F-A92F-4D37-A333-8E83816145B2}" name="Term Accession Number (OBI:0001939)" dataDxfId="10"/>
+    <tableColumn id="46" xr3:uid="{B284403A-6425-4F12-92AD-BF927CA6CE08}" name="Parameter [genome status]" dataDxfId="9"/>
+    <tableColumn id="47" xr3:uid="{E0FF587D-3D23-4C0B-AC12-91911D067572}" name="Term Source REF (DPBO:0000061)" dataDxfId="8"/>
+    <tableColumn id="48" xr3:uid="{77077C0E-6C5B-461E-B8B4-F8EFC42935B8}" name="Term Accession Number (DPBO:0000061)" dataDxfId="7"/>
+    <tableColumn id="49" xr3:uid="{00ECFF3A-1744-44CB-9ADF-2CC0FF569074}" name="Parameter [genome reference sequence]" dataDxfId="6"/>
+    <tableColumn id="50" xr3:uid="{925FA146-4B22-4022-9B72-F9581FE927ED}" name="Term Source REF (DPBO:0000026)" dataDxfId="5"/>
+    <tableColumn id="51" xr3:uid="{08E8013B-595D-4457-8617-D5F7FF7762DD}" name="Term Accession Number (DPBO:0000026)" dataDxfId="4"/>
+    <tableColumn id="52" xr3:uid="{BF863F98-6FFC-4BFA-835F-A6B908BB2D7F}" name="Parameter [processed data file format]" dataDxfId="3"/>
+    <tableColumn id="53" xr3:uid="{D3248941-950E-49FD-AC3A-6C840CBC005D}" name="Term Source REF (DPBO:0000027)" dataDxfId="2"/>
+    <tableColumn id="54" xr3:uid="{10615F06-CF59-4F32-A281-0BD2B35F19E0}" name="Term Accession Number (DPBO:0000027)" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{37AAA820-E44D-492C-A2D8-56248E8B1009}" name="Derived Data File" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1290,53 +1359,53 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AL2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AF21" sqref="AF21"/>
+    <sheetView topLeftCell="W1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="37.44140625" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="32.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.5" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="32.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="31.6640625" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="38.109375" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="38.1640625" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="39.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="31.6640625" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="38.109375" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="42.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="38.1640625" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="42.83203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="31.6640625" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="38.109375" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="53.21875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="38.1640625" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="53.1640625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="31.6640625" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="38.109375" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="39.109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="29.88671875" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="38.1640625" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="39.1640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="29.83203125" hidden="1" customWidth="1"/>
     <col min="19" max="19" width="36.33203125" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="45.77734375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="45.83203125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="31.6640625" hidden="1" customWidth="1"/>
-    <col min="22" max="22" width="38.109375" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="38.1640625" hidden="1" customWidth="1"/>
     <col min="23" max="23" width="35.6640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="29.88671875" hidden="1" customWidth="1"/>
+    <col min="24" max="24" width="29.83203125" hidden="1" customWidth="1"/>
     <col min="25" max="25" width="36.33203125" hidden="1" customWidth="1"/>
-    <col min="26" max="26" width="29.109375" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="29.88671875" hidden="1" customWidth="1"/>
+    <col min="26" max="26" width="29.1640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="29.83203125" hidden="1" customWidth="1"/>
     <col min="28" max="28" width="36.33203125" hidden="1" customWidth="1"/>
     <col min="29" max="29" width="26.33203125" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="31.6640625" hidden="1" customWidth="1"/>
-    <col min="31" max="31" width="38.109375" hidden="1" customWidth="1"/>
+    <col min="31" max="31" width="38.1640625" hidden="1" customWidth="1"/>
     <col min="32" max="32" width="38" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="31.6640625" hidden="1" customWidth="1"/>
-    <col min="34" max="34" width="38.109375" hidden="1" customWidth="1"/>
-    <col min="35" max="35" width="36.109375" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="38.1640625" hidden="1" customWidth="1"/>
+    <col min="35" max="35" width="36.1640625" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="31.6640625" hidden="1" customWidth="1"/>
-    <col min="37" max="37" width="38.109375" hidden="1" customWidth="1"/>
-    <col min="38" max="38" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="38.1640625" hidden="1" customWidth="1"/>
+    <col min="38" max="38" width="17.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1344,46 +1413,46 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E1" t="s">
         <v>105</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G1" t="s">
+        <v>107</v>
+      </c>
+      <c r="H1" t="s">
+        <v>108</v>
+      </c>
+      <c r="I1" t="s">
         <v>109</v>
       </c>
-      <c r="F1" t="s">
+      <c r="J1" t="s">
         <v>110</v>
       </c>
-      <c r="G1" t="s">
+      <c r="K1" t="s">
         <v>111</v>
       </c>
-      <c r="H1" t="s">
+      <c r="L1" t="s">
         <v>112</v>
       </c>
-      <c r="I1" t="s">
+      <c r="M1" t="s">
         <v>113</v>
       </c>
-      <c r="J1" t="s">
+      <c r="N1" t="s">
         <v>114</v>
       </c>
-      <c r="K1" t="s">
+      <c r="O1" t="s">
         <v>115</v>
       </c>
-      <c r="L1" t="s">
+      <c r="P1" t="s">
         <v>116</v>
-      </c>
-      <c r="M1" t="s">
-        <v>117</v>
-      </c>
-      <c r="N1" t="s">
-        <v>118</v>
-      </c>
-      <c r="O1" t="s">
-        <v>119</v>
-      </c>
-      <c r="P1" t="s">
-        <v>120</v>
       </c>
       <c r="Q1" t="s">
         <v>2</v>
@@ -1395,13 +1464,13 @@
         <v>4</v>
       </c>
       <c r="T1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="U1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="V1" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="W1" t="s">
         <v>5</v>
@@ -1422,37 +1491,37 @@
         <v>10</v>
       </c>
       <c r="AC1" t="s">
+        <v>120</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>121</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>122</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>123</v>
+      </c>
+      <c r="AG1" t="s">
         <v>124</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AH1" t="s">
         <v>125</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AI1" t="s">
         <v>126</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AJ1" t="s">
         <v>127</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AK1" t="s">
         <v>128</v>
       </c>
-      <c r="AH1" t="s">
-        <v>129</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>130</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>131</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>132</v>
-      </c>
       <c r="AL1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.3">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:38" x14ac:dyDescent="0.2">
       <c r="B2" s="13"/>
       <c r="C2" s="13" t="s">
         <v>50</v>
@@ -1488,7 +1557,7 @@
         <v>50</v>
       </c>
       <c r="N2" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="O2" s="13" t="s">
         <v>50</v>
@@ -1566,13 +1635,13 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="35.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="57.109375" customWidth="1"/>
+    <col min="2" max="2" width="57.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -1580,7 +1649,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>13</v>
       </c>
@@ -1588,15 +1657,15 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>15</v>
       </c>
@@ -1604,15 +1673,15 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>17</v>
       </c>
@@ -1620,7 +1689,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>18</v>
       </c>
@@ -1628,7 +1697,7 @@
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>19</v>
       </c>
@@ -1640,7 +1709,7 @@
       </c>
       <c r="D8" s="8"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>20</v>
       </c>
@@ -1648,7 +1717,7 @@
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>21</v>
       </c>
@@ -1656,7 +1725,7 @@
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>22</v>
       </c>
@@ -1664,7 +1733,7 @@
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>23</v>
       </c>
@@ -1678,7 +1747,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>24</v>
       </c>
@@ -1686,7 +1755,7 @@
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>25</v>
       </c>
@@ -1694,7 +1763,7 @@
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>26</v>
       </c>
@@ -1702,7 +1771,7 @@
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>27</v>
       </c>
@@ -1716,7 +1785,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>28</v>
       </c>
@@ -1730,7 +1799,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>29</v>
       </c>
@@ -1738,7 +1807,7 @@
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>30</v>
       </c>
@@ -1746,7 +1815,7 @@
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>31</v>
       </c>
@@ -1754,7 +1823,7 @@
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>32</v>
       </c>
@@ -1762,7 +1831,7 @@
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>33</v>
       </c>
@@ -1770,7 +1839,7 @@
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>34</v>
       </c>
@@ -1778,33 +1847,33 @@
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B27" s="9"/>
       <c r="C27" s="9"/>
@@ -1820,27 +1889,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="54.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="46.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>50</v>
       </c>
@@ -1878,7 +1947,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
@@ -1904,7 +1973,7 @@
       <c r="K2" s="12"/>
       <c r="L2" s="12"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
         <v>62</v>
       </c>
@@ -1924,30 +1993,30 @@
         <v>50</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="H3" s="12" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="I3" s="12" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="J3" s="12"/>
       <c r="K3" s="12"/>
       <c r="L3" s="12"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E4" s="12" t="s">
         <v>50</v>
@@ -1956,30 +2025,30 @@
         <v>50</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="H4" s="12" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="I4" s="12" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="J4" s="12"/>
       <c r="K4" s="12"/>
       <c r="L4" s="12"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="E5" s="12" t="s">
         <v>50</v>
@@ -1990,24 +2059,24 @@
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
       <c r="I5" s="12" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="J5" s="12"/>
       <c r="K5" s="12"/>
       <c r="L5" s="12"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="E6" s="12" t="s">
         <v>50</v>
@@ -2018,24 +2087,24 @@
       <c r="G6" s="12"/>
       <c r="H6" s="12"/>
       <c r="I6" s="12" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="J6" s="12"/>
       <c r="K6" s="12"/>
       <c r="L6" s="12"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E7" s="12" t="s">
         <v>50</v>
@@ -2046,24 +2115,24 @@
       <c r="G7" s="12"/>
       <c r="H7" s="12"/>
       <c r="I7" s="12" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="J7" s="12"/>
       <c r="K7" s="12"/>
       <c r="L7" s="12"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E8" s="12" t="s">
         <v>50</v>
@@ -2072,31 +2141,31 @@
         <v>50</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="H8" s="12" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="I8" s="12" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="J8" s="12"/>
       <c r="K8" s="12"/>
       <c r="L8" s="12"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
         <v>2</v>
       </c>
       <c r="B9" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="D9" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="D9" s="12" t="s">
-        <v>66</v>
-      </c>
       <c r="E9" s="12" t="s">
         <v>50</v>
       </c>
@@ -2104,30 +2173,30 @@
         <v>50</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="H9" s="12" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="I9" s="12" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="J9" s="12"/>
       <c r="K9" s="12"/>
       <c r="L9" s="12"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="E10" s="12" t="s">
         <v>50</v>
@@ -2136,31 +2205,31 @@
         <v>50</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="H10" s="12" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="I10" s="12" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="J10" s="12"/>
       <c r="K10" s="12"/>
       <c r="L10" s="12"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
         <v>5</v>
       </c>
       <c r="B11" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="D11" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="C11" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>68</v>
-      </c>
       <c r="E11" s="12" t="s">
         <v>50</v>
       </c>
@@ -2168,31 +2237,31 @@
         <v>50</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="I11" s="12" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="J11" s="12"/>
       <c r="K11" s="12"/>
       <c r="L11" s="12"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="D12" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="C12" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="D12" s="12" t="s">
-        <v>70</v>
-      </c>
       <c r="E12" s="12" t="s">
         <v>50</v>
       </c>
@@ -2200,30 +2269,30 @@
         <v>50</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="H12" s="12" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="I12" s="12" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="J12" s="12"/>
       <c r="K12" s="12"/>
       <c r="L12" s="12"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C13" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="D13" s="14" t="s">
         <v>133</v>
-      </c>
-      <c r="D13" s="14" t="s">
-        <v>137</v>
       </c>
       <c r="E13" s="12" t="s">
         <v>50</v>
@@ -2238,18 +2307,18 @@
       <c r="K13" s="12"/>
       <c r="L13" s="12"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="E14" s="12" t="s">
         <v>50</v>
@@ -2258,30 +2327,30 @@
         <v>50</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="H14" s="12" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="I14" s="12" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="J14" s="12"/>
       <c r="K14" s="12"/>
       <c r="L14" s="12"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="11" t="s">
-        <v>71</v>
+        <v>11</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>72</v>
+        <v>130</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>63</v>
+        <v>129</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>73</v>
+        <v>131</v>
       </c>
       <c r="E15" s="12" t="s">
         <v>50</v>
@@ -2289,42 +2358,36 @@
       <c r="F15" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="G15" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="H15" s="12" t="s">
-        <v>95</v>
-      </c>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
       <c r="I15" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J15" s="12"/>
       <c r="K15" s="12"/>
       <c r="L15" s="12"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="D16" s="14" t="s">
-        <v>135</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="14"/>
       <c r="E16" s="12" t="s">
         <v>50</v>
       </c>
       <c r="F16" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
+      <c r="G16" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="H16" s="12" t="s">
+        <v>91</v>
+      </c>
       <c r="I16" s="12" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="J16" s="12"/>
       <c r="K16" s="12"/>
@@ -2333,15 +2396,14 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D4" r:id="rId1" xr:uid="{70751FB4-3F9A-459E-B046-9B0EECB4A0D8}"/>
-    <hyperlink ref="D15" r:id="rId2" xr:uid="{80587771-CC40-449D-A1D0-49C75D9E77D2}"/>
-    <hyperlink ref="D16" r:id="rId3" xr:uid="{8A285B46-9EA4-4698-B24B-C2B5B2EA1D80}"/>
-    <hyperlink ref="D14" r:id="rId4" xr:uid="{5790CB73-E2F2-445A-BC68-57C899A1A781}"/>
-    <hyperlink ref="D13" r:id="rId5" xr:uid="{3AA6D27E-3C0E-45AD-A5E9-A38E62A0C056}"/>
-    <hyperlink ref="D10" r:id="rId6" xr:uid="{9BF6325D-AC6A-4718-A9F4-5881E7249E90}"/>
-    <hyperlink ref="D8" r:id="rId7" xr:uid="{E590CA81-5DF1-4B93-B5BD-8505F334733D}"/>
-    <hyperlink ref="D7" r:id="rId8" xr:uid="{5A370DF3-F3F8-4802-9881-54DC222DE7A9}"/>
-    <hyperlink ref="D6" r:id="rId9" xr:uid="{92D423C2-EA43-4B2C-873E-695C1FE4368A}"/>
-    <hyperlink ref="D5" r:id="rId10" xr:uid="{B2A3C0E0-5969-4820-B230-D2C4226802A6}"/>
+    <hyperlink ref="D15" r:id="rId2" xr:uid="{8A285B46-9EA4-4698-B24B-C2B5B2EA1D80}"/>
+    <hyperlink ref="D14" r:id="rId3" xr:uid="{5790CB73-E2F2-445A-BC68-57C899A1A781}"/>
+    <hyperlink ref="D13" r:id="rId4" xr:uid="{3AA6D27E-3C0E-45AD-A5E9-A38E62A0C056}"/>
+    <hyperlink ref="D10" r:id="rId5" xr:uid="{9BF6325D-AC6A-4718-A9F4-5881E7249E90}"/>
+    <hyperlink ref="D8" r:id="rId6" xr:uid="{E590CA81-5DF1-4B93-B5BD-8505F334733D}"/>
+    <hyperlink ref="D7" r:id="rId7" xr:uid="{5A370DF3-F3F8-4802-9881-54DC222DE7A9}"/>
+    <hyperlink ref="D6" r:id="rId8" xr:uid="{92D423C2-EA43-4B2C-873E-695C1FE4368A}"/>
+    <hyperlink ref="D5" r:id="rId9" xr:uid="{B2A3C0E0-5969-4820-B230-D2C4226802A6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>